<commit_message>
feat: agregar análisis de bondad de ajuste y actualizar datos de recolección (Frisby)
</commit_message>
<xml_diff>
--- a/RecoleccionDatos.xlsx
+++ b/RecoleccionDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VivoBook\OneDrive\Documentos\Estudios JP\Ingenieria de sistemas\Semestre 6\operaciones\TeoriaColas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD76AC9-C501-425F-8AD9-FB245769DC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD51348-B97F-42C8-A983-DF2B09E114C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -756,7 +756,9 @@
   </sheetPr>
   <dimension ref="A1:M996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3640,25 +3642,25 @@
         <v>70</v>
       </c>
       <c r="B71" s="12">
-        <v>0.5864583333333333</v>
+        <v>0.58646990740740745</v>
       </c>
       <c r="C71" s="13" t="s">
         <v>80</v>
       </c>
       <c r="D71" s="14">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1.0000000000065512</v>
       </c>
       <c r="E71" s="15">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.0000000000065512</v>
       </c>
       <c r="F71" s="16">
         <v>0.60723379629629626</v>
       </c>
       <c r="G71" s="17">
         <f t="shared" si="0"/>
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="H71" s="16">
         <f t="shared" si="1"/>
@@ -3688,11 +3690,11 @@
       </c>
       <c r="D72" s="20">
         <f t="shared" si="4"/>
-        <v>5.000000000003979</v>
+        <v>3.9999999999974278</v>
       </c>
       <c r="E72" s="7">
         <f t="shared" si="5"/>
-        <v>5.000000000003979</v>
+        <v>3.9999999999974278</v>
       </c>
       <c r="F72" s="8">
         <v>0.60802083333333334</v>
@@ -16648,7 +16650,7 @@
   <customSheetViews>
     <customSheetView guid="{394DF760-5100-41DE-A510-FACA521BD004}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:L102" xr:uid="{E2371FFD-7A21-4432-BFA0-88633D30D389}">
+      <autoFilter ref="A1:L102" xr:uid="{B17A85A0-DA98-4469-9DF9-5C23AB80BB85}">
         <filterColumn colId="5">
           <filters>
             <filter val="12:45:20"/>

</xml_diff>